<commit_message>
change xlsx format and build pre task
</commit_message>
<xml_diff>
--- a/Wi-Explorer.xlsx
+++ b/Wi-Explorer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ExplorerTab" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Code</t>
   </si>
@@ -44,41 +44,53 @@
     <t>icon</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>wiToolbar</t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
     <t>wiButton</t>
   </si>
   <si>
-    <t>help_32x32</t>
-  </si>
-  <si>
-    <t>info_frp_32x32</t>
-  </si>
-  <si>
-    <t>Toolbar</t>
-  </si>
-  <si>
-    <t>ExplorerButton1Button</t>
-  </si>
-  <si>
-    <t>ExplorerButton2Button</t>
-  </si>
-  <si>
-    <t>ExplorerButton3Button</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Image Name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>project_new_32x32</t>
+  </si>
+  <si>
+    <t>project_open_32x32</t>
+  </si>
+  <si>
+    <t>project_close_32x32</t>
+  </si>
+  <si>
+    <t>DatabasesToolbar</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>NewProjectButton</t>
+  </si>
+  <si>
+    <t>OpenProjectButton</t>
+  </si>
+  <si>
+    <t>CloseProjectButton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,8 +98,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +135,18 @@
         <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -110,10 +157,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -124,8 +173,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,16 +458,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -425,62 +483,71 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10" t="str">
+        <f>REPLACE(C2, 1, 2, "")</f>
+        <v>Toolbar</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="H2" t="str">
-        <f>REPLACE(C2,1,2,"")</f>
-        <v>Toolbar</v>
-      </c>
-      <c r="I2">
-        <f>LEN(H2)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+      <c r="D3" t="str">
+        <f>REPLACE(C3, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
       <c r="F3" t="str">
-        <f>SUBSTITUTE(J3,"_","-")</f>
-        <v>help-32x32</v>
-      </c>
-      <c r="H3" t="str">
-        <f>REPLACE(C3,1,2,"")</f>
-        <v>Button</v>
-      </c>
-      <c r="I3">
-        <f>LEN(H3)</f>
-        <v>6</v>
+        <f>SUBSTITUTE(E3,"_","-")</f>
+        <v>project-new-32x32</v>
       </c>
       <c r="J3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -488,25 +555,24 @@
         <v>1.2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D5" si="0">REPLACE(C4, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="F4" t="str">
-        <f>SUBSTITUTE(J4,"_","-")</f>
-        <v>info-frp-32x32</v>
-      </c>
-      <c r="H4" t="str">
-        <f>REPLACE(C4,1,2,"")</f>
-        <v>Button</v>
-      </c>
-      <c r="I4">
-        <f>LEN(H4)</f>
-        <v>6</v>
+        <f t="shared" ref="F4:F5" si="1">SUBSTITUTE(E4,"_","-")</f>
+        <v>project-open-32x32</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -514,23 +580,43 @@
         <v>1.3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
       </c>
       <c r="F5" t="str">
-        <f>SUBSTITUTE(J5,"_","-")</f>
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <f>REPLACE(C5,1,2,"")</f>
-        <v>Button</v>
-      </c>
-      <c r="I5">
-        <f>LEN(H5)</f>
-        <v>6</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>project-close-32x32</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
set icon wi-logplot and wi-explorer
</commit_message>
<xml_diff>
--- a/Wi-Explorer.xlsx
+++ b/Wi-Explorer.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TooNies1810/Documents/lab/ribon-angular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ExplorerTab" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Code</t>
   </si>
@@ -59,15 +54,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>project_new_32x32</t>
-  </si>
-  <si>
-    <t>project_open_32x32</t>
-  </si>
-  <si>
-    <t>project_close_32x32</t>
-  </si>
-  <si>
     <t>DatabasesToolbar</t>
   </si>
   <si>
@@ -77,13 +63,61 @@
     <t>small</t>
   </si>
   <si>
-    <t>NewProjectButton</t>
-  </si>
-  <si>
-    <t>OpenProjectButton</t>
-  </si>
-  <si>
-    <t>CloseProjectButton</t>
+    <t>ImportProjectButton</t>
+  </si>
+  <si>
+    <t>wiDropdown</t>
+  </si>
+  <si>
+    <t>import_file</t>
+  </si>
+  <si>
+    <t>ReloadProjectButton</t>
+  </si>
+  <si>
+    <t>CollapseProjectButton</t>
+  </si>
+  <si>
+    <t>DeleteProjectButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wiButton </t>
+  </si>
+  <si>
+    <t>BrowseProjectButton</t>
+  </si>
+  <si>
+    <t>reload_16x16</t>
+  </si>
+  <si>
+    <t>apply_16x16</t>
+  </si>
+  <si>
+    <t>browse_project</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>Reload</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Browse project</t>
+  </si>
+  <si>
+    <t>delete_16x16</t>
+  </si>
+  <si>
+    <t>Image inactive</t>
+  </si>
+  <si>
+    <t>delete_inactive_16x16/</t>
   </si>
 </sst>
 </file>
@@ -162,7 +196,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -179,6 +213,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -238,7 +276,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -273,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -450,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,21 +496,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,15 +540,18 @@
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -525,62 +567,68 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D3" t="str">
         <f>REPLACE(C3, 1, 2, "")</f>
-        <v>Button</v>
+        <v>Dropdown</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F3" t="str">
         <f>SUBSTITUTE(E3,"_","-")</f>
-        <v>project-new-32x32</v>
+        <v>import-file</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1.2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D5" si="0">REPLACE(C4, 1, 2, "")</f>
+        <f t="shared" ref="D4:D7" si="0">REPLACE(C4, 1, 2, "")</f>
         <v>Button</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F5" si="1">SUBSTITUTE(E4,"_","-")</f>
-        <v>project-open-32x32</v>
+        <f t="shared" ref="F4:F7" si="1">SUBSTITUTE(E4,"_","-")</f>
+        <v>reload-16x16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1.3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -590,32 +638,91 @@
         <v>Button</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
-        <v>project-close-32x32</v>
+        <v>apply-16x16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Button </v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>delete-16x16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Button </v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>browse-project</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update wi-logplot and wi-explorer
</commit_message>
<xml_diff>
--- a/Wi-Explorer.xlsx
+++ b/Wi-Explorer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Code</t>
   </si>
@@ -63,9 +63,6 @@
     <t>small</t>
   </si>
   <si>
-    <t>ImportProjectButton</t>
-  </si>
-  <si>
     <t>wiDropdown</t>
   </si>
   <si>
@@ -118,6 +115,102 @@
   </si>
   <si>
     <t>delete_inactive_16x16/</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>ImportProjectDropdown</t>
+  </si>
+  <si>
+    <t>ImportASCIIButton</t>
+  </si>
+  <si>
+    <t>ImportMultiASCIIButton</t>
+  </si>
+  <si>
+    <t>ImportLASButton</t>
+  </si>
+  <si>
+    <t>ImportMultiLASButton</t>
+  </si>
+  <si>
+    <t>ImportDLISButton</t>
+  </si>
+  <si>
+    <t>Interval/CoreLoaderButton</t>
+  </si>
+  <si>
+    <t>MultiWellCoreLoaderButton</t>
+  </si>
+  <si>
+    <t>ImportWellHeaderButton</t>
+  </si>
+  <si>
+    <t>ImportWellTopButton</t>
+  </si>
+  <si>
+    <t>ascii_import_16x16</t>
+  </si>
+  <si>
+    <t>las_import_16x16</t>
+  </si>
+  <si>
+    <t>load_16x16</t>
+  </si>
+  <si>
+    <t>Import ASCII</t>
+  </si>
+  <si>
+    <t>Import Multi ASCII</t>
+  </si>
+  <si>
+    <t>Import LAS</t>
+  </si>
+  <si>
+    <t>Import Multi LAS</t>
+  </si>
+  <si>
+    <t>Import DLIS</t>
+  </si>
+  <si>
+    <t>Interval/Core Loader</t>
+  </si>
+  <si>
+    <t>Multi Well Core Loader</t>
+  </si>
+  <si>
+    <t>Import Well Header</t>
+  </si>
+  <si>
+    <t>Import Well Top</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>1.1.6</t>
+  </si>
+  <si>
+    <t>1.1.7</t>
+  </si>
+  <si>
+    <t>1.1.8</t>
+  </si>
+  <si>
+    <t>1.1.9</t>
   </si>
 </sst>
 </file>
@@ -156,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +274,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4A506"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -196,7 +295,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -217,6 +316,16 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -488,7 +597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,15 +605,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
@@ -543,7 +652,7 @@
         <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -567,163 +676,412 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="str">
+      <c r="D3" s="16" t="str">
         <f>REPLACE(C3, 1, 2, "")</f>
         <v>Dropdown</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="str">
+      <c r="E3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="16" t="str">
         <f>SUBSTITUTE(E3,"_","-")</f>
         <v>import-file</v>
       </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" ref="D4:D7" si="0">REPLACE(C4, 1, 2, "")</f>
+      <c r="D4" s="7" t="str">
+        <f t="shared" ref="D4:D12" si="0">REPLACE(C4, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" ref="F4:F7" si="1">SUBSTITUTE(E4,"_","-")</f>
-        <v>reload-16x16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
+      <c r="E4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="7" t="str">
+        <f t="shared" ref="F4:F12" si="1">SUBSTITUTE(E4,"_","-")</f>
+        <v>ascii-import-16x16</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="5" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Button</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>ascii-import-16x16</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>las-import-16x16</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>las-import-16x16</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>load-16x16</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>load-16x16</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>las-import-16x16</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Button</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>las-import-16x16</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:D16" si="2">REPLACE(C13, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13:F16" si="3">SUBSTITUTE(E13,"_","-")</f>
+        <v>reload-16x16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>Button</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v>apply-16x16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">Button </v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v>delete-16x16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">Button </v>
+      </c>
+      <c r="E16" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="1"/>
-        <v>apply-16x16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Button </v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="1"/>
-        <v>delete-16x16</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v>browse-project</v>
+      </c>
+      <c r="G16" t="s">
         <v>28</v>
       </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">Button </v>
-      </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v>browse-project</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
disable/ enable dropdown ribbon, explorer
</commit_message>
<xml_diff>
--- a/Wi-Explorer.xlsx
+++ b/Wi-Explorer.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
   <si>
     <t>Code</t>
   </si>
@@ -71,9 +71,6 @@
     <t>wiDropdown</t>
   </si>
   <si>
-    <t>import_file</t>
-  </si>
-  <si>
     <t>ReloadProjectButton</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>apply_16x16</t>
   </si>
   <si>
-    <t>browse_project</t>
-  </si>
-  <si>
     <t>Import</t>
   </si>
   <si>
@@ -225,6 +219,9 @@
   </si>
   <si>
     <t>explorer</t>
+  </si>
+  <si>
+    <t>project_new_16x16</t>
   </si>
 </sst>
 </file>
@@ -623,7 +620,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="93" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -670,13 +667,13 @@
         <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -701,18 +698,18 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>14</v>
@@ -722,31 +719,31 @@
         <v>Dropdown</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="F3" s="16" t="str">
         <f>SUBSTITUTE(E3,"_","-")</f>
-        <v>import-file</v>
+        <v>project-new-16x16</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>7</v>
@@ -756,31 +753,31 @@
         <v>Button</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F4" s="7" t="str">
         <f t="shared" ref="F4:F12" si="1">SUBSTITUTE(E4,"_","-")</f>
         <v>ascii-import-16x16</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>7</v>
@@ -790,31 +787,31 @@
         <v>Button</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ascii-import-16x16</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>7</v>
@@ -824,31 +821,31 @@
         <v>Button</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>las-import-16x16</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>7</v>
@@ -858,31 +855,31 @@
         <v>Button</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>las-import-16x16</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
         <v>13</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>7</v>
@@ -896,24 +893,24 @@
         <v/>
       </c>
       <c r="G8" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
         <v>13</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>7</v>
@@ -923,31 +920,31 @@
         <v>Button</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>load-16x16</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M9" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>7</v>
@@ -957,31 +954,31 @@
         <v>Button</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>load-16x16</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
         <v>13</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M10" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>7</v>
@@ -991,31 +988,31 @@
         <v>Button</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>las-import-16x16</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J11" t="s">
         <v>13</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>7</v>
@@ -1025,23 +1022,23 @@
         <v>Button</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>las-import-16x16</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
         <v>13</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1049,7 +1046,7 @@
         <v>1.2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1059,7 +1056,7 @@
         <v>Button</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ref="F13:F16" si="3">SUBSTITUTE(E13,"_","-")</f>
@@ -1069,13 +1066,13 @@
         <v>13</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1083,7 +1080,7 @@
         <v>1.3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -1093,7 +1090,7 @@
         <v>Button</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="3"/>
@@ -1103,13 +1100,13 @@
         <v>13</v>
       </c>
       <c r="K14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M14" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1117,17 +1114,17 @@
         <v>1.4</v>
       </c>
       <c r="B15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
         <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">Button </v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="3"/>
@@ -1137,13 +1134,13 @@
         <v>13</v>
       </c>
       <c r="K15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M15" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1151,33 +1148,33 @@
         <v>1.5</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">Button </v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="3"/>
-        <v>browse-project</v>
+        <v>project-new-16x16</v>
       </c>
       <c r="J16" t="s">
         <v>13</v>
       </c>
       <c r="K16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M16" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>